<commit_message>
feat: JFrame, 주석 추가
</commit_message>
<xml_diff>
--- a/src/main/java/db/LectureRoomReservation.xlsx
+++ b/src/main/java/db/LectureRoomReservation.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgzza\OneDrive\바탕 화면\과제\소프트웨어 공학\LectureRoomReservation\src\main\java\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4329330D-E275-4120-95B2-9791CE5894B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F1AB5F-5825-49B6-A1C1-3E7F734FB70A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{CD724C36-E040-4A9B-8DAC-BE65BDB47C58}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{CD724C36-E040-4A9B-8DAC-BE65BDB47C58}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="67">
   <si>
     <t>이름</t>
   </si>
@@ -74,12 +74,6 @@
     <t>강의실이 너무 더럽다.</t>
   </si>
   <si>
-    <t>321</t>
-  </si>
-  <si>
-    <t>김광식</t>
-  </si>
-  <si>
     <t>예약 번호</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -115,13 +109,188 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>911-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>911-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>915-12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>916-18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>916-20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>917-34</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>918-40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>abc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>def</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ghi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jkl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mno</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pqr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tuv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wxy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zzz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>non</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>uwu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nwn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>owo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ouo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>abcd1234</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>efgh5678</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ijkl9101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mnop1213</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qrst1415</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>uvwx1617</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yzzz1819</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>afsj1234</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adsf1230</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zvhj2940</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>oijq1592</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>saog2408</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hdzo1987</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zcxv3498</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>xovi2349</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2025.05.11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2025.05.12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2025.05.13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2025.05.20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2025.05.21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2025.06.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2025.07.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -161,8 +330,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -487,70 +659,70 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="0">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="F1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s" s="0">
+      <c r="G1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s" s="0">
+      <c r="G2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
         <v>22</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s" s="0">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -562,17 +734,52 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F3C8A87-E491-4391-AB43-3743AF995DCE}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A1" t="s" s="0">
-        <v>21</v>
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -583,36 +790,337 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB5E0FD-E9D4-4434-BA57-5E4432659AA5}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="5" max="5" customWidth="true" width="19.3984375"/>
-    <col min="6" max="6" customWidth="true" width="14.69921875"/>
+    <col min="4" max="4" width="10.59765625" customWidth="1"/>
+    <col min="5" max="5" width="19.3984375" customWidth="1"/>
+    <col min="6" max="6" width="14.69921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="D1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="E1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="F1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s" s="0">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>19</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
         <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.45833333333333331</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>58</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>67</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0.875</v>
       </c>
     </row>
   </sheetData>
@@ -631,28 +1139,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="5" max="5" customWidth="true" width="21.3984375"/>
-    <col min="6" max="6" customWidth="true" width="13.59765625"/>
+    <col min="5" max="5" width="21.3984375" customWidth="1"/>
+    <col min="6" max="6" width="13.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="D1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="E1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="F1" t="s">
         <v>18</v>
-      </c>
-      <c r="E1" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="F1" t="s" s="0">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -671,28 +1179,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="5" max="5" customWidth="true" width="20.19921875"/>
-    <col min="6" max="6" customWidth="true" width="14.19921875"/>
+    <col min="5" max="5" width="20.19921875" customWidth="1"/>
+    <col min="6" max="6" width="14.19921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="D1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="E1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="F1" t="s">
         <v>18</v>
-      </c>
-      <c r="E1" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="F1" t="s" s="0">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -711,28 +1219,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="5" max="5" customWidth="true" width="22.0"/>
-    <col min="6" max="6" customWidth="true" width="13.796875"/>
+    <col min="5" max="5" width="22" customWidth="1"/>
+    <col min="6" max="6" width="13.796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="D1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="E1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="F1" t="s">
         <v>18</v>
-      </c>
-      <c r="E1" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="F1" t="s" s="0">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -751,28 +1259,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="5" max="5" customWidth="true" width="21.09765625"/>
-    <col min="6" max="6" customWidth="true" width="13.0"/>
+    <col min="5" max="5" width="21.09765625" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="D1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="E1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="F1" t="s">
         <v>18</v>
-      </c>
-      <c r="E1" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="F1" t="s" s="0">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -791,28 +1299,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="5" max="5" customWidth="true" width="22.3984375"/>
-    <col min="6" max="6" customWidth="true" width="13.5"/>
+    <col min="5" max="5" width="22.3984375" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="D1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="E1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="F1" t="s">
         <v>18</v>
-      </c>
-      <c r="E1" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="F1" t="s" s="0">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -831,28 +1339,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="5" max="5" customWidth="true" width="21.296875"/>
-    <col min="6" max="6" customWidth="true" width="15.296875"/>
+    <col min="5" max="5" width="21.296875" customWidth="1"/>
+    <col min="6" max="6" width="15.296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="D1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="E1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="F1" t="s">
         <v>18</v>
-      </c>
-      <c r="E1" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="F1" t="s" s="0">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>